<commit_message>
time rising from <20 threads
</commit_message>
<xml_diff>
--- a/zarzadz-threads.xlsx
+++ b/zarzadz-threads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovooo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD192467-F6CC-4AD2-A738-440EA5146ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2183E14-0755-4E6D-8253-60C5DA16DC72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{8A5ADEEA-BEDF-4E9D-A33A-9D91EFBB0F45}"/>
   </bookViews>
@@ -86,14 +86,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -109,6 +110,1997 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>17 cities</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$A$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$A$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.6559489999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6926130000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0167027</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99998139999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94023910999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0571493999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0867720000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8A21-4964-BAE5-8B2E474496BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="500641552"/>
+        <c:axId val="500647456"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="500641552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="500647456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="500647456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="500641552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>20 cities</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$K$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$K$13:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>85.398399999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.937540000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.912040000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.433009999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.02783</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.073879999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CEC-4D72-8A30-C07CD985021C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="501866408"/>
+        <c:axId val="501862472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="501866408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501862472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="501862472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="501866408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9AB7A93-7BB7-4721-A6C6-58FE7AA71125}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBFF8044-0313-4B2F-964A-FC5D4E9D2640}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,34 +2403,34 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -503,6 +2495,12 @@
       <c r="E3">
         <v>0.83859499999999998</v>
       </c>
+      <c r="F3">
+        <v>0.82258399999999998</v>
+      </c>
+      <c r="G3">
+        <v>1.08277</v>
+      </c>
       <c r="K3">
         <v>88.421899999999994</v>
       </c>
@@ -514,6 +2512,12 @@
       </c>
       <c r="N3">
         <v>11.305999999999999</v>
+      </c>
+      <c r="O3" s="5">
+        <v>13.2834</v>
+      </c>
+      <c r="P3">
+        <v>12.8962</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -532,6 +2536,12 @@
       <c r="E4">
         <v>0.83559099999999997</v>
       </c>
+      <c r="F4">
+        <v>1.02973</v>
+      </c>
+      <c r="G4">
+        <v>1.08077</v>
+      </c>
       <c r="K4">
         <v>94.247</v>
       </c>
@@ -543,6 +2553,12 @@
       </c>
       <c r="N4">
         <v>11.278</v>
+      </c>
+      <c r="O4" s="5">
+        <v>11.8985</v>
+      </c>
+      <c r="P4">
+        <v>11.9655</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -561,6 +2577,12 @@
       <c r="E5">
         <v>0.82658699999999996</v>
       </c>
+      <c r="F5">
+        <v>1.0857699999999999</v>
+      </c>
+      <c r="G5">
+        <v>1.08077</v>
+      </c>
       <c r="K5">
         <v>92.970100000000002</v>
       </c>
@@ -572,6 +2594,12 @@
       </c>
       <c r="N5">
         <v>11.308</v>
+      </c>
+      <c r="O5" s="5">
+        <v>11.8864</v>
+      </c>
+      <c r="P5">
+        <v>11.9755</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -590,6 +2618,12 @@
       <c r="E6">
         <v>0.83658999999999994</v>
       </c>
+      <c r="F6">
+        <v>1.10178</v>
+      </c>
+      <c r="G6">
+        <v>1.0817699999999999</v>
+      </c>
       <c r="K6">
         <v>84.502099999999999</v>
       </c>
@@ -601,6 +2635,12 @@
       </c>
       <c r="N6">
         <v>11.321</v>
+      </c>
+      <c r="O6" s="5">
+        <v>12.0185</v>
+      </c>
+      <c r="P6">
+        <v>11.919499999999999</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -619,6 +2659,12 @@
       <c r="E7">
         <v>0.84151909999999996</v>
       </c>
+      <c r="F7">
+        <v>1.08477</v>
+      </c>
+      <c r="G7">
+        <v>1.09077</v>
+      </c>
       <c r="K7">
         <v>60.905999999999999</v>
       </c>
@@ -630,6 +2676,12 @@
       </c>
       <c r="N7">
         <v>11.279</v>
+      </c>
+      <c r="O7" s="5">
+        <v>11.824400000000001</v>
+      </c>
+      <c r="P7">
+        <v>12.000500000000001</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -648,6 +2700,12 @@
       <c r="E8">
         <v>1.1188</v>
       </c>
+      <c r="F8">
+        <v>1.0897699999999999</v>
+      </c>
+      <c r="G8">
+        <v>1.09778</v>
+      </c>
       <c r="K8">
         <v>58.679699999999997</v>
       </c>
@@ -659,6 +2717,12 @@
       </c>
       <c r="N8">
         <v>11.266</v>
+      </c>
+      <c r="O8" s="5">
+        <v>11.823399999999999</v>
+      </c>
+      <c r="P8">
+        <v>12.0395</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -677,6 +2741,12 @@
       <c r="E9">
         <v>0.833592</v>
       </c>
+      <c r="F9">
+        <v>1.09378</v>
+      </c>
+      <c r="G9">
+        <v>1.0817699999999999</v>
+      </c>
       <c r="K9">
         <v>91.997399999999999</v>
       </c>
@@ -688,6 +2758,12 @@
       </c>
       <c r="N9">
         <v>12.64</v>
+      </c>
+      <c r="O9" s="5">
+        <v>11.807399999999999</v>
+      </c>
+      <c r="P9">
+        <v>11.952500000000001</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -706,6 +2782,12 @@
       <c r="E10">
         <v>1.6</v>
       </c>
+      <c r="F10">
+        <v>1.0877699999999999</v>
+      </c>
+      <c r="G10">
+        <v>1.10178</v>
+      </c>
       <c r="K10">
         <v>94.750299999999996</v>
       </c>
@@ -717,6 +2799,12 @@
       </c>
       <c r="N10">
         <v>11.3581</v>
+      </c>
+      <c r="O10" s="5">
+        <v>11.888400000000001</v>
+      </c>
+      <c r="P10">
+        <v>12.099600000000001</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -735,6 +2823,12 @@
       <c r="E11">
         <v>0.82951900000000001</v>
       </c>
+      <c r="F11">
+        <v>1.08677</v>
+      </c>
+      <c r="G11">
+        <v>1.08277</v>
+      </c>
       <c r="K11">
         <v>95.087599999999995</v>
       </c>
@@ -746,6 +2840,12 @@
       </c>
       <c r="N11">
         <v>11.271000000000001</v>
+      </c>
+      <c r="O11" s="5">
+        <v>11.993499999999999</v>
+      </c>
+      <c r="P11">
+        <v>11.9495</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -764,6 +2864,12 @@
       <c r="E12">
         <v>0.84159799999999996</v>
       </c>
+      <c r="F12">
+        <v>1.08877</v>
+      </c>
+      <c r="G12">
+        <v>1.08677</v>
+      </c>
       <c r="K12">
         <v>92.421899999999994</v>
       </c>
@@ -776,55 +2882,77 @@
       <c r="N12">
         <v>11.303000000000001</v>
       </c>
+      <c r="O12" s="5">
+        <v>11.8544</v>
+      </c>
+      <c r="P12">
+        <v>11.9405</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <f>SUM(A3:A12)/10</f>
         <v>8.6559489999999997</v>
       </c>
-      <c r="B13" s="3">
-        <f t="shared" ref="B13:E13" si="0">SUM(B3:B12)/10</f>
+      <c r="B13" s="2">
+        <f t="shared" ref="B13:G13" si="0">SUM(B3:B12)/10</f>
         <v>2.6926130000000001</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>1.0167027</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <f>SUM(D3:D12)/10</f>
         <v>0.99998139999999991</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>0.94023910999999993</v>
       </c>
-      <c r="K13" s="4">
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0571493999999999</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0867720000000001</v>
+      </c>
+      <c r="K13" s="3">
         <f>SUM(K3:K12)/10</f>
         <v>85.398399999999995</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="3">
         <f>SUM(L3:L12)/10</f>
         <v>19.937540000000002</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <f>SUM(M3:M12)/10</f>
         <v>11.912040000000001</v>
       </c>
-      <c r="N13" s="4">
-        <f t="shared" ref="M13:N13" si="1">SUM(N3:N12)/10</f>
+      <c r="N13" s="3">
+        <f t="shared" ref="N13:P13" si="1">SUM(N3:N12)/10</f>
         <v>11.433009999999999</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="1"/>
+        <v>12.02783</v>
+      </c>
+      <c r="P13" s="3">
+        <f t="shared" si="1"/>
+        <v>12.073879999999999</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -833,5 +2961,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>